<commit_message>
sudah membuat logic gugus
</commit_message>
<xml_diff>
--- a/public/DataMahasiswa/datamahasiswa.xlsx
+++ b/public/DataMahasiswa/datamahasiswa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\OneDrive\Documents\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD938401-D43F-4E46-9249-64BA29584B69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36BDB44A-3282-4EB4-A35F-F23D26956BF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C787810A-3289-4AB3-97F6-F74C27BF23BB}"/>
   </bookViews>
@@ -418,7 +418,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -461,7 +461,7 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2">
         <v>2023</v>
@@ -481,7 +481,7 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <v>2023</v>
@@ -541,7 +541,7 @@
         <v>1</v>
       </c>
       <c r="E6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6">
         <v>2023</v>
@@ -561,7 +561,7 @@
         <v>1</v>
       </c>
       <c r="E7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7">
         <v>2023</v>

</xml_diff>